<commit_message>
Vijay's Latest code for Opp,GiftLogs,TimeRecorManager
</commit_message>
<xml_diff>
--- a/TestData/Outlook.xlsx
+++ b/TestData/Outlook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HL\SalesForce_Project\SalesForce_Project\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3397D5A7-D13D-4BEA-804D-38E6A9A5CA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81CFF48-FE81-4F4D-8A0A-EB6810A1DA1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCredential" sheetId="2" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>Sahil.Mittal0207@hl.com</t>
+    <t>vkumar0427@hl.com</t>
   </si>
   <si>
-    <t>Yankee@12345</t>
+    <t>Angeles$2023</t>
   </si>
 </sst>
 </file>
@@ -377,16 +377,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -394,7 +394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -405,7 +405,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId2" display="Yankee@12345" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes to TMTT0017339_EventExpense_VerifyTheCFExpenseRequestFunctionalityAsApprover - 21 Dec 2023
</commit_message>
<xml_diff>
--- a/TestData/Outlook.xlsx
+++ b/TestData/Outlook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vkumar0427\source\repos\SF_Automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81CFF48-FE81-4F4D-8A0A-EB6810A1DA1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EFAE0B-30E6-4C4D-ABEB-D6874FF25418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UserCredential" sheetId="2" r:id="rId1"/>
@@ -33,10 +33,10 @@
     <t>UserName</t>
   </si>
   <si>
-    <t>vkumar0427@hl.com</t>
+    <t>Sahil.Mittal0207@hl.com</t>
   </si>
   <si>
-    <t>Angeles$2023</t>
+    <t>Yankee@123456</t>
   </si>
 </sst>
 </file>
@@ -377,16 +377,16 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -394,7 +394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -405,7 +405,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" display="Yankee@12345" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{F5C72CA9-FBBC-45C0-9CC7-C43A4301B8D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Outlook login cred update - 4 Dec 2024
</commit_message>
<xml_diff>
--- a/TestData/Outlook.xlsx
+++ b/TestData/Outlook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EFAE0B-30E6-4C4D-ABEB-D6874FF25418}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C796D8FA-38A3-49A3-BBFB-8D64620D624A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
     <t>Sahil.Mittal0207@hl.com</t>
   </si>
   <si>
-    <t>Yankee@123456</t>
+    <t>Welcome241029</t>
   </si>
 </sst>
 </file>
@@ -377,7 +377,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -405,7 +405,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{F5C72CA9-FBBC-45C0-9CC7-C43A4301B8D3}"/>
+    <hyperlink ref="B2" r:id="rId2" display="Yankee@123456" xr:uid="{F5C72CA9-FBBC-45C0-9CC7-C43A4301B8D3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>